<commit_message>
- I2C clock speed now adjustable - IP address and port now stored in eeprom
</commit_message>
<xml_diff>
--- a/Comm_Protocol.xlsx
+++ b/Comm_Protocol.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="83">
   <si>
     <t>LM35</t>
   </si>
@@ -106,33 +106,15 @@
     <t>PWM_HLT</t>
   </si>
   <si>
-    <t>TBOIL</t>
-  </si>
-  <si>
-    <t>TCFC</t>
-  </si>
-  <si>
-    <t>FLOW3</t>
-  </si>
-  <si>
-    <t>FLOW4</t>
-  </si>
-  <si>
     <t>V3.30</t>
   </si>
   <si>
     <t>0..16, value</t>
   </si>
   <si>
-    <t>WB</t>
-  </si>
-  <si>
     <t>PWM_BOIL</t>
   </si>
   <si>
-    <t>WH</t>
-  </si>
-  <si>
     <t>pwm_2_time</t>
   </si>
   <si>
@@ -263,13 +245,34 @@
   </si>
   <si>
     <t>owc_task</t>
+  </si>
+  <si>
+    <t>0..6, value</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>H x B x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1 S2 S3 </t>
+  </si>
+  <si>
+    <t>Temperatures</t>
+  </si>
+  <si>
+    <t>Flows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +291,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -321,19 +332,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,9 +396,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -405,9 +430,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,9 +465,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -614,17 +641,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AA49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -654,36 +681,36 @@
     <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
       <c r="L2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="2:27">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K3">
         <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="M3">
         <v>50</v>
@@ -692,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Q3">
         <v>50</v>
@@ -700,7 +727,7 @@
       <c r="X3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="2:27">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
@@ -710,17 +737,20 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="K4">
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -729,7 +759,7 @@
         <v>30</v>
       </c>
       <c r="P4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Q4">
         <v>2000</v>
@@ -737,24 +767,25 @@
       <c r="X4" s="4"/>
       <c r="AA4" s="4"/>
     </row>
-    <row r="5" spans="2:27">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="K5">
         <v>50</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="M5">
         <v>1000</v>
@@ -767,54 +798,48 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
     </row>
-    <row r="6" spans="2:27">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <v>2</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="3">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="K6">
         <v>60</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O6">
         <v>60</v>
       </c>
       <c r="P6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
     </row>
-    <row r="7" spans="2:27">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <v>3</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="3">
-        <v>3</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="K7">
         <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M7">
         <v>1000</v>
@@ -824,57 +849,51 @@
       </c>
       <c r="X7" s="4"/>
     </row>
-    <row r="8" spans="2:27">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="3">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="K8">
         <v>110</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O8">
         <v>110</v>
       </c>
       <c r="P8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="X8" s="4"/>
     </row>
-    <row r="9" spans="2:27">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>5</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="3">
-        <v>5</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="K9">
         <v>160</v>
       </c>
       <c r="L9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O9" s="4">
         <v>120</v>
       </c>
       <c r="P9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="Q9">
         <v>1000</v>
@@ -884,82 +903,73 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
     </row>
-    <row r="10" spans="2:27">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <v>6</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="3">
-        <v>6</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="K10">
         <v>210</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O10">
         <v>160</v>
       </c>
       <c r="P10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
     </row>
-    <row r="11" spans="2:27">
-      <c r="F11" s="3">
-        <v>7</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>31</v>
-      </c>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="K11">
         <v>260</v>
       </c>
       <c r="L11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O11">
         <v>210</v>
       </c>
       <c r="P11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="X11" s="4"/>
     </row>
-    <row r="12" spans="2:27">
-      <c r="F12" s="3">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>32</v>
-      </c>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="K12">
         <v>310</v>
       </c>
       <c r="L12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O12" s="4">
         <v>220</v>
       </c>
       <c r="P12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="Q12">
         <v>1000</v>
       </c>
       <c r="AA12" s="4"/>
     </row>
-    <row r="13" spans="2:27">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
@@ -969,6 +979,9 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
+      <c r="E13" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
@@ -979,7 +992,7 @@
         <v>320</v>
       </c>
       <c r="L13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M13">
         <v>1000</v>
@@ -988,13 +1001,14 @@
         <v>260</v>
       </c>
       <c r="P13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="2:27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <v>1</v>
       </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="2">
         <v>1</v>
       </c>
@@ -1002,16 +1016,16 @@
         <v>360</v>
       </c>
       <c r="L14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O14">
         <v>310</v>
       </c>
       <c r="P14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="2:27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1021,6 +1035,9 @@
       <c r="D15" t="s">
         <v>9</v>
       </c>
+      <c r="E15" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
@@ -1031,22 +1048,23 @@
         <v>410</v>
       </c>
       <c r="L15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O15">
         <v>320</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="Q15">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="2:27">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <v>1</v>
       </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="2">
         <v>1</v>
       </c>
@@ -1054,7 +1072,7 @@
         <v>420</v>
       </c>
       <c r="L16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M16">
         <v>1000</v>
@@ -1063,21 +1081,24 @@
         <v>360</v>
       </c>
       <c r="P16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
+      <c r="E17" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="F17" s="2" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
@@ -1086,16 +1107,16 @@
         <v>460</v>
       </c>
       <c r="L17" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O17">
         <v>410</v>
       </c>
       <c r="P17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1105,6 +1126,9 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
+      <c r="E18" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F18" s="2">
         <v>0</v>
       </c>
@@ -1115,22 +1139,23 @@
         <v>510</v>
       </c>
       <c r="L18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O18">
         <v>420</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q18">
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="2:17">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <v>1</v>
       </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="2">
         <v>1</v>
       </c>
@@ -1138,7 +1163,7 @@
         <v>520</v>
       </c>
       <c r="L19" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M19">
         <v>2000</v>
@@ -1147,10 +1172,10 @@
         <v>460</v>
       </c>
       <c r="P19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1160,6 +1185,9 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
+      <c r="E20" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="F20" s="2">
         <v>0</v>
       </c>
@@ -1170,22 +1198,23 @@
         <v>560</v>
       </c>
       <c r="L20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O20">
         <v>510</v>
       </c>
       <c r="P20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>19</v>
       </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="2">
         <v>1</v>
       </c>
@@ -1196,25 +1225,26 @@
         <v>610</v>
       </c>
       <c r="L21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O21">
         <v>520</v>
       </c>
       <c r="P21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="Q21">
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="2:17">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <v>2</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
       </c>
+      <c r="E22" s="5"/>
       <c r="F22" s="2">
         <v>2</v>
       </c>
@@ -1225,7 +1255,7 @@
         <v>620</v>
       </c>
       <c r="L22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1234,16 +1264,17 @@
         <v>560</v>
       </c>
       <c r="P22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <v>3</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="2">
         <v>3</v>
       </c>
@@ -1254,22 +1285,23 @@
         <v>660</v>
       </c>
       <c r="L23" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O23">
         <v>610</v>
       </c>
       <c r="P23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <v>4</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
       </c>
+      <c r="E24" s="5"/>
       <c r="F24" s="2">
         <v>4</v>
       </c>
@@ -1280,19 +1312,19 @@
         <v>710</v>
       </c>
       <c r="L24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O24">
         <v>620</v>
       </c>
       <c r="P24" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="Q24">
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="2:17">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1302,6 +1334,9 @@
       <c r="D25" t="s">
         <v>25</v>
       </c>
+      <c r="E25" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="F25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1312,16 +1347,16 @@
         <v>760</v>
       </c>
       <c r="L25" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O25">
         <v>660</v>
       </c>
       <c r="P25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1331,406 +1366,406 @@
       <c r="D26" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>35</v>
+      <c r="E26" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="K26">
         <v>810</v>
       </c>
       <c r="L26" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O26">
         <v>710</v>
       </c>
       <c r="P26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17">
-      <c r="E27" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E27" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K27">
         <v>860</v>
       </c>
       <c r="L27" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O27">
         <v>760</v>
       </c>
       <c r="P27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K28">
         <v>910</v>
       </c>
       <c r="L28" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O28">
         <v>810</v>
       </c>
       <c r="P28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K29">
         <v>960</v>
       </c>
       <c r="L29" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O29">
         <v>860</v>
       </c>
       <c r="P29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="O30">
         <v>910</v>
       </c>
       <c r="P30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="O31">
         <v>960</v>
       </c>
       <c r="P31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33"/>
       <c r="C33" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D34">
         <v>2000</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F34" s="4">
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H34">
         <v>2000</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D35">
         <v>2000</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F35" s="4">
         <v>50</v>
       </c>
       <c r="G35" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H35">
         <v>2000</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D36">
         <v>1000</v>
       </c>
       <c r="E36" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F36" s="4">
         <v>100</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H36" s="4">
         <v>2000</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>270</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D37">
         <v>1000</v>
       </c>
       <c r="E37" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F37" s="4">
         <v>150</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H37" s="4">
         <v>2000</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>180</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D38">
         <v>1000</v>
       </c>
       <c r="E38" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F38" s="4">
         <v>200</v>
       </c>
       <c r="G38" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H38">
         <v>1000</v>
       </c>
       <c r="I38" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J38" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>270</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D39">
         <v>1000</v>
       </c>
       <c r="E39" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F39" s="4">
         <v>250</v>
       </c>
       <c r="G39" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H39">
         <v>1000</v>
       </c>
       <c r="I39" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>360</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D40">
         <v>2000</v>
       </c>
       <c r="E40" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F40" s="4">
         <v>300</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H40" s="4">
         <v>1000</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>450</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D41">
         <v>20000</v>
       </c>
       <c r="E41" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F41" s="4">
         <v>350</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H41" s="4">
         <v>1000</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>470</v>
       </c>
       <c r="C42" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D42">
         <v>500</v>
       </c>
       <c r="E42" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F42" s="4">
         <v>400</v>
       </c>
       <c r="G42" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H42">
         <v>2000</v>
       </c>
       <c r="I42" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>490</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D43">
         <v>1000</v>
       </c>
       <c r="E43" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F43">
         <v>450</v>
       </c>
       <c r="G43" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H43">
         <v>20000</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="2:10">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>520</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D44">
         <v>5000</v>
@@ -1739,139 +1774,139 @@
         <v>470</v>
       </c>
       <c r="G44" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H44">
         <v>500</v>
       </c>
       <c r="I44" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J44" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>540</v>
       </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D45">
         <v>5000</v>
       </c>
       <c r="E45" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F45">
         <v>490</v>
       </c>
       <c r="G45" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H45">
         <v>1000</v>
       </c>
       <c r="I45" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="J45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>600</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D46">
         <v>1000</v>
       </c>
       <c r="E46" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F46">
         <v>520</v>
       </c>
       <c r="G46" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H46">
         <v>5000</v>
       </c>
     </row>
-    <row r="47" spans="2:10">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>970</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D47">
         <v>500</v>
       </c>
       <c r="E47" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F47">
         <v>540</v>
       </c>
       <c r="G47" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H47">
         <v>5000</v>
       </c>
       <c r="I47" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J47" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48"/>
       <c r="C48"/>
       <c r="F48">
         <v>600</v>
       </c>
       <c r="G48" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H48">
         <v>1000</v>
       </c>
       <c r="I48" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49"/>
       <c r="C49"/>
       <c r="F49">
         <v>970</v>
       </c>
       <c r="G49" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H49">
         <v>500</v>
       </c>
       <c r="I49" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J49" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.44" right="0.54" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="69" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="69" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>